<commit_message>
Update(JDT) : Journal de travail du Mardi 28 octobre
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_VicheryAaron.xlsx
+++ b/Journal-de-Travail_VicheryAaron.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2eme\Modules\Module 320\Projet\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F953D8-F4CA-491A-913A-3090B2507A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93A4839-8B8A-4429-88A4-18AA5F1F5EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="825" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -161,6 +161,21 @@
   </si>
   <si>
     <t>Essayer d'ajouter la fonction pour déplacer le personnage</t>
+  </si>
+  <si>
+    <t>Ajouter les obstacles dans mon jeu</t>
+  </si>
+  <si>
+    <t>Faire le déplacement des ennemis et des obstacles</t>
+  </si>
+  <si>
+    <t>J'ai oublié de le faire la semaine avant les vacances et le lundi 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essayer de faire les collisions entre le projectile et l'ennemi ou l'obstacle </t>
+  </si>
+  <si>
+    <t>Afficher le score dans la console</t>
   </si>
 </sst>
 </file>
@@ -616,6 +631,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="16" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -625,10 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,7 +1190,7 @@
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2027,16 +2042,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.43373493975903615</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36144578313253012</c:v>
+                  <c:v>0.57936507936507942</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20481927710843373</c:v>
+                  <c:v>0.13492063492063491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4220,9 +4235,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4254,28 +4269,28 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="84" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="64"/>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="86"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 55 minutes</v>
+        <v>10 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4288,24 +4303,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>235</v>
+        <v>270</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>415</v>
+        <v>630</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="86"/>
     </row>
     <row r="6" spans="1:15" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -4547,7 +4562,7 @@
       <c r="F14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="87"/>
+      <c r="G14" s="84"/>
       <c r="N14">
         <v>7</v>
       </c>
@@ -4591,66 +4606,104 @@
       <c r="D16" s="32"/>
       <c r="E16" s="33"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="39"/>
+      <c r="G16" s="39" t="s">
+        <v>42</v>
+      </c>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="str">
+      <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B17" s="34">
+        <v>45958</v>
+      </c>
       <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="23"/>
+      <c r="D17" s="36">
+        <v>20</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="G17" s="40"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="str">
+      <c r="A18" s="62">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45958</v>
+      </c>
+      <c r="C18" s="31">
+        <v>2</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="G18" s="39"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45958</v>
+      </c>
+      <c r="C19" s="35">
+        <v>1</v>
+      </c>
+      <c r="D19" s="36">
+        <v>0</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="str">
+      <c r="A20" s="62">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B20" s="30">
+        <v>45958</v>
+      </c>
       <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
+      <c r="D20" s="32">
+        <v>15</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -4675,7 +4728,7 @@
       <c r="D22" s="32"/>
       <c r="E22" s="33"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="87"/>
+      <c r="G22" s="84"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="str">
@@ -10956,7 +11009,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.43373493975903615</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10973,15 +11026,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>365</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10989,11 +11042,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>2 h 30 min</v>
+        <v>6 h 05 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.36144578313253012</v>
+        <v>0.57936507936507942</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11067,7 +11120,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.20481927710843373</v>
+        <v>0.13492063492063491</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11119,26 +11172,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>235</v>
+        <v>270</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>415</v>
+        <v>630</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 55 min</v>
+        <v>10 h 30 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>7.6851851851851852E-2</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11182,15 +11235,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B1120F001D1794FAA6F4057E3355991" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a3fb6df6b31548c4fd074caa2ed14580">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f20a0681-8b2f-4a46-9dab-cf1520193f81" xmlns:ns3="932fafb7-d8e0-4a14-bee3-33aad5c71309" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d4691fe5d3e52a7f10faf36b21998c3" ns2:_="" ns3:_="">
     <xsd:import namespace="f20a0681-8b2f-4a46-9dab-cf1520193f81"/>
@@ -11379,6 +11423,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11391,14 +11444,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B1176-FD39-41C7-AFE3-BD9EE39B178A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11417,6 +11462,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update(JDT): Ajout de ce que j'ai fait aujourd'hui dans mon JDT
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_VicheryAaron.xlsx
+++ b/Journal-de-Travail_VicheryAaron.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93A4839-8B8A-4429-88A4-18AA5F1F5EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024E0B08-6DDC-412C-AF7B-D265E5009D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Afficher le score dans la console</t>
+  </si>
+  <si>
+    <t>Ajouter les collisions</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1193,7 @@
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>365</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1263,7 +1266,6 @@
     </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1271,6 +1273,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1610,7 +1613,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1618,6 +1620,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2042,16 +2045,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.2857142857142857</c:v>
+                  <c:v>0.24827586206896551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57936507936507942</c:v>
+                  <c:v>0.6344827586206897</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13492063492063491</c:v>
+                  <c:v>0.11724137931034483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2206,7 +2209,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2214,6 +2216,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4237,7 +4240,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4290,7 +4293,7 @@
       <c r="B3" s="87"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>10 heures 30 minutes</v>
+        <v>12 heures 5 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4303,15 +4306,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>270</v>
+        <v>305</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>630</v>
+        <v>725</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4707,15 +4710,25 @@
       <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="str">
+      <c r="A21" s="63">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B21" s="34">
+        <v>45959</v>
+      </c>
+      <c r="C21" s="35">
+        <v>1</v>
+      </c>
+      <c r="D21" s="36">
+        <v>35</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -11009,7 +11022,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.2857142857142857</v>
+        <v>0.24827586206896551</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11026,15 +11039,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>460</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11042,11 +11055,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>6 h 05 min</v>
+        <v>7 h 40 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.57936507936507942</v>
+        <v>0.6344827586206897</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11120,7 +11133,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.13492063492063491</v>
+        <v>0.11724137931034483</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11172,26 +11185,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>270</v>
+        <v>305</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>630</v>
+        <v>725</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>10 h 30 min</v>
+        <v>12 h 05 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.11666666666666667</v>
+        <v>0.13425925925925927</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11235,6 +11248,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f20a0681-8b2f-4a46-9dab-cf1520193f81">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="932fafb7-d8e0-4a14-bee3-33aad5c71309" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B1120F001D1794FAA6F4057E3355991" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a3fb6df6b31548c4fd074caa2ed14580">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f20a0681-8b2f-4a46-9dab-cf1520193f81" xmlns:ns3="932fafb7-d8e0-4a14-bee3-33aad5c71309" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d4691fe5d3e52a7f10faf36b21998c3" ns2:_="" ns3:_="">
     <xsd:import namespace="f20a0681-8b2f-4a46-9dab-cf1520193f81"/>
@@ -11423,27 +11456,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f20a0681-8b2f-4a46-9dab-cf1520193f81"/>
+    <ds:schemaRef ds:uri="932fafb7-d8e0-4a14-bee3-33aad5c71309"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f20a0681-8b2f-4a46-9dab-cf1520193f81">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="932fafb7-d8e0-4a14-bee3-33aad5c71309" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B1176-FD39-41C7-AFE3-BD9EE39B178A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11460,23 +11492,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f20a0681-8b2f-4a46-9dab-cf1520193f81"/>
-    <ds:schemaRef ds:uri="932fafb7-d8e0-4a14-bee3-33aad5c71309"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update(JDT) : Ajout de ce que j'ai fait aujourd'hui dans mon JDT
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_VicheryAaron.xlsx
+++ b/Journal-de-Travail_VicheryAaron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024E0B08-6DDC-412C-AF7B-D265E5009D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293B3438-0C37-4D24-AF48-E657A30C9AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -178,7 +178,10 @@
     <t>Afficher le score dans la console</t>
   </si>
   <si>
-    <t>Ajouter les collisions</t>
+    <t>Ajouter les collisions dans mon jeu</t>
+  </si>
+  <si>
+    <t>Ajouter les conditions de victoire et de défaite</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1196,7 @@
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>460</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2045,16 +2048,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.24827586206896551</c:v>
+                  <c:v>0.22929936305732485</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6344827586206897</c:v>
+                  <c:v>0.66242038216560506</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724137931034483</c:v>
+                  <c:v>0.10828025477707007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4238,9 +4241,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4293,7 +4296,7 @@
       <c r="B3" s="87"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>12 heures 5 minutes</v>
+        <v>13 heures 5 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4306,7 +4309,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -4314,7 +4317,7 @@
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>725</v>
+        <v>785</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4732,15 +4735,25 @@
       <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="str">
+      <c r="A22" s="62">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B22" s="30">
+        <v>45959</v>
+      </c>
+      <c r="C22" s="31">
+        <v>1</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="G22" s="84"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -11022,7 +11035,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.24827586206896551</v>
+        <v>0.22929936305732485</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11039,7 +11052,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
@@ -11047,7 +11060,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>460</v>
+        <v>520</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11055,11 +11068,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>7 h 40 min</v>
+        <v>8 h 40 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.6344827586206897</v>
+        <v>0.66242038216560506</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11133,7 +11146,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.11724137931034483</v>
+        <v>0.10828025477707007</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11185,7 +11198,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
@@ -11193,18 +11206,18 @@
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>725</v>
+        <v>785</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>12 h 05 min</v>
+        <v>13 h 05 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.13425925925925927</v>
+        <v>0.14537037037037037</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11248,6 +11261,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="f20a0681-8b2f-4a46-9dab-cf1520193f81">
@@ -11256,15 +11278,6 @@
     <TaxCatchAll xmlns="932fafb7-d8e0-4a14-bee3-33aad5c71309" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11457,20 +11470,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f20a0681-8b2f-4a46-9dab-cf1520193f81"/>
     <ds:schemaRef ds:uri="932fafb7-d8e0-4a14-bee3-33aad5c71309"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update(JDT) : Ajout de ce que j'ai fait le 31 octobre
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_VicheryAaron.xlsx
+++ b/Journal-de-Travail_VicheryAaron.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293B3438-0C37-4D24-AF48-E657A30C9AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D755974-86B0-426F-A894-2DA6297B67C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t>Ajouter les conditions de victoire et de défaite</t>
+  </si>
+  <si>
+    <t>Ajout de tous les commentaires dans mon code</t>
+  </si>
+  <si>
+    <t>Ajout des maquettes pour mes user stories dans mon projet sur github</t>
+  </si>
+  <si>
+    <t>Continuer mon rapport</t>
   </si>
 </sst>
 </file>
@@ -449,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -637,10 +646,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="16" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1193,16 +1198,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>180</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>520</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1269,6 +1274,7 @@
     </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1276,7 +1282,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1616,6 +1621,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1623,7 +1629,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2048,16 +2053,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.22929936305732485</c:v>
+                  <c:v>0.21546961325966851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66242038216560506</c:v>
+                  <c:v>0.64088397790055252</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10828025477707007</c:v>
+                  <c:v>0.143646408839779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2212,6 +2217,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2219,7 +2225,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4242,8 +4247,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4275,28 +4280,28 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="85" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="64"/>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="87"/>
+      <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>13 heures 5 minutes</v>
+        <v>15 heures 5 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4309,24 +4314,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>480</v>
+        <v>540</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>305</v>
+        <v>365</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>785</v>
+        <v>905</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="86"/>
+      <c r="D5" s="85"/>
     </row>
     <row r="6" spans="1:15" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -4568,7 +4573,7 @@
       <c r="F14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="84"/>
+      <c r="G14" s="39"/>
       <c r="N14">
         <v>7</v>
       </c>
@@ -4754,42 +4759,68 @@
       <c r="F22" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="84"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="str">
+      <c r="A23" s="63">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B23" s="34">
+        <v>45961</v>
+      </c>
+      <c r="C23" s="35">
+        <v>1</v>
+      </c>
+      <c r="D23" s="36">
+        <v>0</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="str">
+      <c r="A24" s="62">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B24" s="30">
+        <v>45961</v>
+      </c>
       <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="23"/>
+      <c r="D24" s="32">
+        <v>15</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>48</v>
+      </c>
       <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="str">
+      <c r="A25" s="63">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B25" s="34">
+        <v>45961</v>
+      </c>
       <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="23"/>
+      <c r="D25" s="36">
+        <v>45</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -11019,11 +11050,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">SUM(A6:B6)</f>
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E6" s="70" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11031,11 +11062,11 @@
       </c>
       <c r="F6" s="71" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>3 h 00 min</v>
+        <v>3 h 15 min</v>
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.22929936305732485</v>
+        <v>0.21546961325966851</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11052,7 +11083,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
@@ -11060,7 +11091,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>520</v>
+        <v>580</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11068,11 +11099,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>8 h 40 min</v>
+        <v>9 h 40 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.66242038216560506</v>
+        <v>0.64088397790055252</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11130,11 +11161,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11142,11 +11173,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 25 min</v>
+        <v>2 h 10 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.10828025477707007</v>
+        <v>0.143646408839779</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11198,26 +11229,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>480</v>
+        <v>540</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>305</v>
+        <v>365</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>785</v>
+        <v>905</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>13 h 05 min</v>
+        <v>15 h 05 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.14537037037037037</v>
+        <v>0.1675925925925926</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11261,15 +11292,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="f20a0681-8b2f-4a46-9dab-cf1520193f81">
@@ -11278,6 +11300,15 @@
     <TaxCatchAll xmlns="932fafb7-d8e0-4a14-bee3-33aad5c71309" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11470,20 +11501,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f20a0681-8b2f-4a46-9dab-cf1520193f81"/>
     <ds:schemaRef ds:uri="932fafb7-d8e0-4a14-bee3-33aad5c71309"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>